<commit_message>
Add Excel output formatting and clean Python-to-Excel pipeline
</commit_message>
<xml_diff>
--- a/dcf_inputs.xlsx
+++ b/dcf_inputs.xlsx
@@ -1,118 +1,56 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
-  <workbookPr defaultThemeVersion="202300"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rabag\OneDrive\Desktop\automated-dcf\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8B3B443-5AFF-471F-A700-B347EA616FC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-23220" yWindow="1500" windowWidth="21600" windowHeight="11505" xr2:uid="{6F2315E4-2DB9-49AC-B562-BBC0335C933A}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-23220" yWindow="1500" windowWidth="21600" windowHeight="11505" tabRatio="600" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="inputs" sheetId="1" r:id="rId1"/>
+    <sheet name="inputs" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="output" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <definedNames/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
-  <si>
-    <t>Ticker</t>
-  </si>
-  <si>
-    <t>AAPL</t>
-  </si>
-  <si>
-    <t>WACC</t>
-  </si>
-  <si>
-    <t>Terminal Growth</t>
-  </si>
-  <si>
-    <t>Tax Rate</t>
-  </si>
-  <si>
-    <t>Forecast Years</t>
-  </si>
-  <si>
-    <t>D&amp;A %</t>
-  </si>
-  <si>
-    <t>CapEx %</t>
-  </si>
-  <si>
-    <t>NWC %</t>
-  </si>
-  <si>
-    <t>Cash</t>
-  </si>
-  <si>
-    <t>Debt</t>
-  </si>
-  <si>
-    <t>Shares Outstanding</t>
-  </si>
-  <si>
-    <t>WACC Range</t>
-  </si>
-  <si>
-    <t>Terminal g Range</t>
-  </si>
-  <si>
-    <t>0.08,0.085,0.09,0.095,0.10</t>
-  </si>
-  <si>
-    <t>0.02,0.025,0.03</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="$#,##0"/>
+    <numFmt numFmtId="165" formatCode="$#,##0.00"/>
+  </numFmts>
+  <fonts count="4">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <name val="Arial Unicode MS"/>
+      <color theme="1"/>
       <sz val="10"/>
-      <color theme="1"/>
-      <name val="Arial Unicode MS"/>
+    </font>
+    <font>
+      <name val="Aptos Narrow"/>
+      <b val="1"/>
+      <sz val="11"/>
+    </font>
+    <font>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -120,27 +58,115 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+  <cellXfs count="6">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -460,124 +486,215 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F3EEE17-2572-44DA-A2B5-BE06266537A3}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A2:B17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col width="18.5703125" bestFit="1" customWidth="1" min="1" max="1"/>
+    <col width="23.5703125" bestFit="1" customWidth="1" min="2" max="2"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:2">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3">
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Ticker</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>AAPL</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>WACC</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
         <v>0.09</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
-      <c r="A4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4">
-        <v>2.5000000000000001E-2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5">
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Terminal Growth</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>0.025</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Tax Rate</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
         <v>0.25</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
-      <c r="A6" t="s">
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Forecast Years</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
         <v>5</v>
       </c>
-      <c r="B6">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7">
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>D&amp;A %</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
         <v>0.03</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
-      <c r="A8" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8">
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>CapEx %</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
         <v>0.04</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
-      <c r="A9" t="s">
-        <v>8</v>
-      </c>
-      <c r="B9">
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>NWC %</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
         <v>0.02</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
-      <c r="A12" t="s">
-        <v>9</v>
-      </c>
-      <c r="B12">
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Cash</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
         <v>10000000000</v>
       </c>
     </row>
-    <row r="13" spans="1:2">
-      <c r="A13" t="s">
-        <v>10</v>
-      </c>
-      <c r="B13" s="1">
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Debt</t>
+        </is>
+      </c>
+      <c r="B13" s="1" t="n">
         <v>50000000000</v>
       </c>
     </row>
-    <row r="14" spans="1:2">
-      <c r="A14" t="s">
-        <v>11</v>
-      </c>
-      <c r="B14">
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Shares Outstanding</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
         <v>16000000000</v>
       </c>
     </row>
-    <row r="16" spans="1:2">
-      <c r="A16" t="s">
-        <v>12</v>
-      </c>
-      <c r="B16" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2">
-      <c r="A17" t="s">
-        <v>13</v>
-      </c>
-      <c r="B17" t="s">
-        <v>15</v>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>WACC Range</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>0.08,0.085,0.09,0.095,0.10</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Terminal g Range</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>0.02,0.025,0.03</t>
+        </is>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="21" customWidth="1" min="1" max="1"/>
+    <col width="19" customWidth="1" min="2" max="2"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="3" t="inlineStr">
+        <is>
+          <t>Metric</t>
+        </is>
+      </c>
+      <c r="B1" s="3" t="inlineStr">
+        <is>
+          <t>Value</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>enterprise_value</t>
+        </is>
+      </c>
+      <c r="B2" s="4" t="n">
+        <v>1288876028868.884</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>implied_share_price</t>
+        </is>
+      </c>
+      <c r="B3" s="5" t="n">
+        <v>78.05475180430525</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Export and format DCF sensitivity table to Excel
</commit_message>
<xml_diff>
--- a/dcf_inputs.xlsx
+++ b/dcf_inputs.xlsx
@@ -3,11 +3,12 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-23220" yWindow="1500" windowWidth="21600" windowHeight="11505" tabRatio="600" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-22875" yWindow="1845" windowWidth="21600" windowHeight="11505" tabRatio="600" firstSheet="0" activeTab="2" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="inputs" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="output" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="sensitivity" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
@@ -16,9 +17,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="$#,##0"/>
-    <numFmt numFmtId="165" formatCode="$#,##0.00"/>
+  <numFmts count="4">
+    <numFmt numFmtId="164" formatCode="\$#,##0"/>
+    <numFmt numFmtId="165" formatCode="\$#,##0.00"/>
+    <numFmt numFmtId="166" formatCode="$#,##0"/>
+    <numFmt numFmtId="167" formatCode="$#,##0.00"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -83,17 +86,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -497,7 +502,7 @@
       <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
     <col width="18.5703125" bestFit="1" customWidth="1" min="1" max="1"/>
     <col width="23.5703125" bestFit="1" customWidth="1" min="2" max="2"/>
@@ -656,19 +661,19 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
     <col width="21" customWidth="1" min="1" max="1"/>
     <col width="19" customWidth="1" min="2" max="2"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="3" t="inlineStr">
+      <c r="A1" s="5" t="inlineStr">
         <is>
           <t>Metric</t>
         </is>
       </c>
-      <c r="B1" s="3" t="inlineStr">
+      <c r="B1" s="5" t="inlineStr">
         <is>
           <t>Value</t>
         </is>
@@ -680,7 +685,7 @@
           <t>enterprise_value</t>
         </is>
       </c>
-      <c r="B2" s="4" t="n">
+      <c r="B2" s="6" t="n">
         <v>1288876028868.884</v>
       </c>
     </row>
@@ -690,11 +695,129 @@
           <t>implied_share_price</t>
         </is>
       </c>
-      <c r="B3" s="5" t="n">
+      <c r="B3" s="7" t="n">
         <v>78.05475180430525</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="7" customWidth="1" min="1" max="1"/>
+    <col width="19" customWidth="1" min="2" max="2"/>
+    <col width="19" customWidth="1" min="3" max="3"/>
+    <col width="19" customWidth="1" min="4" max="4"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="5" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="C1" s="5" t="n">
+        <v>0.025</v>
+      </c>
+      <c r="D1" s="5" t="n">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="5" t="n">
+        <v>0.08</v>
+      </c>
+      <c r="B2" s="6" t="n">
+        <v>1419861275649.4</v>
+      </c>
+      <c r="C2" s="6" t="n">
+        <v>1522496183431.889</v>
+      </c>
+      <c r="D2" s="6" t="n">
+        <v>1645658072770.875</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="5" t="n">
+        <v>0.08500000000000001</v>
+      </c>
+      <c r="B3" s="6" t="n">
+        <v>1310699804072.444</v>
+      </c>
+      <c r="C3" s="6" t="n">
+        <v>1395954929662.583</v>
+      </c>
+      <c r="D3" s="6" t="n">
+        <v>1496710987178.202</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="5" t="n">
+        <v>0.09</v>
+      </c>
+      <c r="B4" s="6" t="n">
+        <v>1217131849916.936</v>
+      </c>
+      <c r="C4" s="6" t="n">
+        <v>1288876028868.884</v>
+      </c>
+      <c r="D4" s="6" t="n">
+        <v>1372577570979.49</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="5" t="n">
+        <v>0.095</v>
+      </c>
+      <c r="B5" s="6" t="n">
+        <v>1136038731263.724</v>
+      </c>
+      <c r="C5" s="6" t="n">
+        <v>1197089098141.867</v>
+      </c>
+      <c r="D5" s="6" t="n">
+        <v>1267531829155.108</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="5" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="B6" s="6" t="n">
+        <v>1065081436092.523</v>
+      </c>
+      <c r="C6" s="6" t="n">
+        <v>1117535853428.621</v>
+      </c>
+      <c r="D6" s="6" t="n">
+        <v>1177483758955.591</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="B2:D6">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="00F8696B"/>
+        <color rgb="00FFEB84"/>
+        <color rgb="0063BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>